<commit_message>
Requirements y archivo xlsx
</commit_message>
<xml_diff>
--- a/sales_2021.xlsx
+++ b/sales_2021.xlsx
@@ -16,8 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +29,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -52,17 +61,20 @@
       <bottom style="thin"/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -134,6 +146,236 @@
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <style val="2"/>
+  <chart>
+    <title>
+      <tx>
+        <rich>
+          <a:bodyPr/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:t>Ventas</a:t>
+            </a:r>
+          </a:p>
+        </rich>
+      </tx>
+    </title>
+    <plotArea>
+      <barChart>
+        <barDir val="col"/>
+        <grouping val="clustered"/>
+        <ser>
+          <idx val="0"/>
+          <order val="0"/>
+          <tx>
+            <strRef>
+              <f>'Report'!B5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$B$6:$B$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="1"/>
+          <order val="1"/>
+          <tx>
+            <strRef>
+              <f>'Report'!C5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$C$6:$C$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="2"/>
+          <order val="2"/>
+          <tx>
+            <strRef>
+              <f>'Report'!D5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$D$6:$D$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="3"/>
+          <order val="3"/>
+          <tx>
+            <strRef>
+              <f>'Report'!E5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$E$6:$E$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="4"/>
+          <order val="4"/>
+          <tx>
+            <strRef>
+              <f>'Report'!F5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$F$6:$F$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <ser>
+          <idx val="5"/>
+          <order val="5"/>
+          <tx>
+            <strRef>
+              <f>'Report'!G5</f>
+            </strRef>
+          </tx>
+          <spPr>
+            <a:ln>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </spPr>
+          <cat>
+            <numRef>
+              <f>'Report'!$B$6:$A$7</f>
+            </numRef>
+          </cat>
+          <val>
+            <numRef>
+              <f>'Report'!$G$6:$G$7</f>
+            </numRef>
+          </val>
+        </ser>
+        <gapWidth val="150"/>
+        <axId val="10"/>
+        <axId val="100"/>
+      </barChart>
+      <catAx>
+        <axId val="10"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="100"/>
+        <lblOffset val="100"/>
+      </catAx>
+      <valAx>
+        <axId val="100"/>
+        <scaling>
+          <orientation val="minMax"/>
+        </scaling>
+        <axPos val="l"/>
+        <majorGridlines/>
+        <majorTickMark val="none"/>
+        <minorTickMark val="none"/>
+        <crossAx val="10"/>
+      </valAx>
+    </plotArea>
+    <legend>
+      <legendPos val="r"/>
+    </legend>
+    <plotVisOnly val="1"/>
+    <dispBlanksAs val="gap"/>
+  </chart>
+</chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
+      <row>11</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="5400000" cy="2700000"/>
+    <graphicFrame>
+      <nvGraphicFramePr>
+        <cNvPr id="1" name="Chart 1"/>
+        <cNvGraphicFramePr/>
+      </nvGraphicFramePr>
+      <xfrm/>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </graphicFrame>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -420,12 +662,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A5:G7"/>
+  <dimension ref="A5:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -520,7 +762,14 @@
         <v>26548</v>
       </c>
     </row>
+    <row r="8">
+      <c r="B8" s="2">
+        <f>SUM(B6:B7)</f>
+        <v/>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>